<commit_message>
Updated logging output format
</commit_message>
<xml_diff>
--- a/stats/analysis/individual.xlsx
+++ b/stats/analysis/individual.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\plough\stats\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/git/plough/stats/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC859FBA-9D26-444E-9BC7-39B1A5FD0E41}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="15495" xr2:uid="{CFED1120-0F4A-4315-9196-CDC886DDA9DC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340"/>
   </bookViews>
   <sheets>
     <sheet name="Batting - 2018" sheetId="1" r:id="rId1"/>
     <sheet name="Bowling - 2018" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="95">
   <si>
     <t>Matches</t>
   </si>
   <si>
-    <t>Innings</t>
-  </si>
-  <si>
-    <t>Not Outs</t>
-  </si>
-  <si>
     <t>Runs</t>
   </si>
   <si>
@@ -51,18 +50,12 @@
     <t>Strike Rate</t>
   </si>
   <si>
-    <t>High Score</t>
-  </si>
-  <si>
     <t>50s</t>
   </si>
   <si>
     <t>100s</t>
   </si>
   <si>
-    <t>Ducks</t>
-  </si>
-  <si>
     <t>Fours</t>
   </si>
   <si>
@@ -301,12 +294,39 @@
   </si>
   <si>
     <t>Low (9-11) (%)</t>
+  </si>
+  <si>
+    <t>Mat</t>
+  </si>
+  <si>
+    <t>Inns</t>
+  </si>
+  <si>
+    <t>Ave</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>0s</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>4s</t>
+  </si>
+  <si>
+    <t>6s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -388,7 +408,7 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -397,14 +417,14 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -413,26 +433,26 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -445,7 +465,7 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -454,11 +474,11 @@
         <color rgb="FFDDDDDD"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -466,33 +486,33 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -510,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -564,17 +584,25 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -582,14 +610,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -903,91 +929,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F0B605-0F06-4362-8C62-80F6A2C61BFD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
         <v>2018</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="18"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="J6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="9" t="s">
+      <c r="K6" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="M6" s="36" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>12</v>
       </c>
       <c r="B7" s="14">
         <v>19</v>
@@ -1008,7 +1040,7 @@
         <v>62.42</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I7" s="7">
         <v>4</v>
@@ -1026,9 +1058,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
         <v>12</v>
@@ -1050,7 +1082,7 @@
         <v>70</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I8" s="2">
         <v>3</v>
@@ -1068,9 +1100,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B9" s="4">
         <v>7</v>
@@ -1109,9 +1141,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2">
         <v>10</v>
@@ -1132,7 +1164,7 @@
         <v>60</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I10" s="2">
         <v>2</v>
@@ -1150,9 +1182,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B11" s="4">
         <v>9</v>
@@ -1191,27 +1223,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M12" s="11"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1226,68 +1258,68 @@
       <c r="L15" s="3"/>
       <c r="M15" s="13"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="1" t="s">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="E19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="G19" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="B22" s="32" t="s">
         <v>36</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>40</v>
       </c>
       <c r="C22" s="32"/>
       <c r="D22" s="32"/>
@@ -1295,436 +1327,436 @@
       <c r="F22" s="32"/>
       <c r="G22" s="32"/>
       <c r="H22" s="32"/>
-      <c r="I22" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="J22" s="31" t="s">
+      <c r="I22" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="L22" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="K22" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="L22" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="M22" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="N22" s="31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M22" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="N22" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>43211</v>
       </c>
-      <c r="B23" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
+      <c r="B23" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
       <c r="I23" s="20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J23" s="21">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22">
         <v>43218</v>
       </c>
-      <c r="B24" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
+      <c r="B24" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
       <c r="I24" s="23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J24" s="24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>43232</v>
       </c>
-      <c r="B25" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
+      <c r="B25" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
       <c r="I25" s="20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J25" s="21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22">
         <v>43240</v>
       </c>
-      <c r="B26" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
+      <c r="B26" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
       <c r="I26" s="23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J26" s="24">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>43246</v>
       </c>
-      <c r="B27" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
+      <c r="B27" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
       <c r="I27" s="20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J27" s="21">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22">
         <v>43253</v>
       </c>
-      <c r="B28" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
+      <c r="B28" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
       <c r="I28" s="23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J28" s="24">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="19">
         <v>43254</v>
       </c>
-      <c r="B29" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
+      <c r="B29" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
       <c r="I29" s="20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J29" s="21">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22">
         <v>43267</v>
       </c>
-      <c r="B30" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
+      <c r="B30" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
       <c r="I30" s="23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J30" s="24">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
         <v>43268</v>
       </c>
-      <c r="B31" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
+      <c r="B31" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
       <c r="I31" s="20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J31" s="21">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22">
         <v>43275</v>
       </c>
-      <c r="B32" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
+      <c r="B32" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
       <c r="I32" s="23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J32" s="24">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="19">
         <v>43281</v>
       </c>
-      <c r="B33" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
+      <c r="B33" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
       <c r="I33" s="20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J33" s="21">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22">
         <v>43288</v>
       </c>
-      <c r="B34" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
+      <c r="B34" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
       <c r="I34" s="23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J34" s="24">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19">
         <v>43295</v>
       </c>
-      <c r="B35" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
+      <c r="B35" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
       <c r="I35" s="20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J35" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22">
         <v>43296</v>
       </c>
-      <c r="B36" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
+      <c r="B36" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
       <c r="I36" s="23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J36" s="24">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19">
         <v>43309</v>
       </c>
-      <c r="B37" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
+      <c r="B37" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
       <c r="I37" s="20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J37" s="21">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22">
         <v>43316</v>
       </c>
-      <c r="B38" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
+      <c r="B38" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
       <c r="I38" s="23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J38" s="24">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="19">
         <v>43317</v>
       </c>
-      <c r="B39" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
+      <c r="B39" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
       <c r="I39" s="20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J39" s="21">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22">
         <v>43324</v>
       </c>
-      <c r="B40" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="26"/>
+      <c r="B40" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
       <c r="I40" s="23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J40" s="24">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19">
         <v>43330</v>
       </c>
-      <c r="B41" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
+      <c r="B41" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
       <c r="I41" s="20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J41" s="21">
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22">
         <v>43337</v>
       </c>
-      <c r="B42" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
+      <c r="B42" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="31"/>
       <c r="I42" s="23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J42" s="24">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="31" t="s">
-        <v>39</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C45" s="32"/>
       <c r="D45" s="32"/>
@@ -1732,63 +1764,70 @@
       <c r="F45" s="32"/>
       <c r="G45" s="32"/>
       <c r="H45" s="32"/>
-      <c r="I45" s="31" t="s">
-        <v>18</v>
+      <c r="I45" s="25" t="s">
+        <v>14</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22">
         <v>43218</v>
       </c>
-      <c r="B46" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26"/>
+      <c r="B46" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="31"/>
       <c r="I46" s="23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J46" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="K46">
         <v>102</v>
       </c>
       <c r="L46" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="M46" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="N46" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
     <mergeCell ref="B41:H41"/>
     <mergeCell ref="B42:H42"/>
     <mergeCell ref="B22:H22"/>
@@ -1805,13 +1844,6 @@
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="B32:H32"/>
     <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1819,91 +1851,91 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE12E9D-DD5B-47E0-A335-F0412F8248AF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
         <v>2018</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="18"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="K6" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="9" t="s">
+      <c r="L6" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="9" t="s">
+      <c r="M6" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="7"/>
@@ -1918,9 +1950,9 @@
       <c r="L7" s="7"/>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1935,9 +1967,9 @@
       <c r="L8" s="2"/>
       <c r="M8" s="5"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1952,9 +1984,9 @@
       <c r="L9" s="4"/>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1969,9 +2001,9 @@
       <c r="L10" s="2"/>
       <c r="M10" s="5"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1986,66 +2018,66 @@
       <c r="L11" s="4"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2054,9 +2086,9 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2065,24 +2097,24 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>89</v>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>85</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2099,7 +2131,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -2107,17 +2139,17 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="31" t="s">
-        <v>39</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C26" s="32"/>
       <c r="D26" s="32"/>
@@ -2125,399 +2157,411 @@
       <c r="F26" s="32"/>
       <c r="G26" s="32"/>
       <c r="H26" s="32"/>
-      <c r="I26" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="J26" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="K26" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="L26" s="31" t="s">
+      <c r="I26" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="L26" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="M26" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="N26" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="O26" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="M26" s="31" t="s">
+      <c r="P26" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="N26" s="9" t="s">
+      <c r="Q26" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="O26" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="P26" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q26" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>43211</v>
       </c>
-      <c r="B27" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
+      <c r="B27" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
       <c r="I27" s="20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J27" s="21"/>
     </row>
-    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22">
         <v>43218</v>
       </c>
-      <c r="B28" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
+      <c r="B28" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
       <c r="I28" s="23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J28" s="24"/>
     </row>
-    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="19">
         <v>43232</v>
       </c>
-      <c r="B29" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
+      <c r="B29" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
       <c r="I29" s="20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J29" s="21"/>
     </row>
-    <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22">
         <v>43240</v>
       </c>
-      <c r="B30" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
+      <c r="B30" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
       <c r="I30" s="23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J30" s="24"/>
     </row>
-    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
         <v>43246</v>
       </c>
-      <c r="B31" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
+      <c r="B31" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
       <c r="I31" s="20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J31" s="21"/>
     </row>
-    <row r="32" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22">
         <v>43253</v>
       </c>
-      <c r="B32" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
+      <c r="B32" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
       <c r="I32" s="23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J32" s="24"/>
     </row>
-    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="19">
         <v>43254</v>
       </c>
-      <c r="B33" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
+      <c r="B33" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
       <c r="I33" s="20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J33" s="21"/>
     </row>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22">
         <v>43267</v>
       </c>
-      <c r="B34" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
+      <c r="B34" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
       <c r="I34" s="23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J34" s="24"/>
     </row>
-    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19">
         <v>43268</v>
       </c>
-      <c r="B35" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
+      <c r="B35" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
       <c r="I35" s="20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J35" s="21"/>
     </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22">
         <v>43275</v>
       </c>
-      <c r="B36" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
+      <c r="B36" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
       <c r="I36" s="23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J36" s="24"/>
     </row>
-    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19">
         <v>43281</v>
       </c>
-      <c r="B37" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
+      <c r="B37" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
       <c r="I37" s="20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J37" s="21"/>
     </row>
-    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22">
         <v>43288</v>
       </c>
-      <c r="B38" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
+      <c r="B38" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
       <c r="I38" s="23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J38" s="24"/>
     </row>
-    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="19">
         <v>43295</v>
       </c>
-      <c r="B39" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
+      <c r="B39" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
       <c r="I39" s="20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J39" s="21"/>
     </row>
-    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22">
         <v>43296</v>
       </c>
-      <c r="B40" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="26"/>
+      <c r="B40" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
       <c r="I40" s="23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J40" s="24"/>
     </row>
-    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19">
         <v>43309</v>
       </c>
-      <c r="B41" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
+      <c r="B41" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
       <c r="I41" s="20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J41" s="21"/>
     </row>
-    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22">
         <v>43316</v>
       </c>
-      <c r="B42" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
+      <c r="B42" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="31"/>
       <c r="I42" s="23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J42" s="24"/>
     </row>
-    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19">
         <v>43317</v>
       </c>
-      <c r="B43" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
+      <c r="B43" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
       <c r="I43" s="20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J43" s="21"/>
     </row>
-    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22">
         <v>43324</v>
       </c>
-      <c r="B44" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="26"/>
+      <c r="B44" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
       <c r="I44" s="23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J44" s="24"/>
     </row>
-    <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19">
         <v>43330</v>
       </c>
-      <c r="B45" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
+      <c r="B45" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
       <c r="I45" s="20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J45" s="21"/>
     </row>
-    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22">
         <v>43337</v>
       </c>
-      <c r="B46" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26"/>
+      <c r="B46" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="31"/>
       <c r="I46" s="23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J46" s="24"/>
     </row>
-    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B37:H37"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B36:H36"/>
     <mergeCell ref="B44:H44"/>
     <mergeCell ref="B45:H45"/>
     <mergeCell ref="B46:H46"/>
@@ -2527,18 +2571,6 @@
     <mergeCell ref="B41:H41"/>
     <mergeCell ref="B42:H42"/>
     <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="B37:H37"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>